<commit_message>
added the formuals in excel page for understanding
</commit_message>
<xml_diff>
--- a/S6/BP_NN_OWN.xlsx
+++ b/S6/BP_NN_OWN.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sriharsha\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ERAV2\S6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{680A003B-9741-4F32-88C1-A4362040DAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1656C8-3602-46A9-9873-602284D0B4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{20ABD9D6-099D-4511-830E-A4E388347D91}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>t1</t>
   </si>
@@ -133,12 +133,39 @@
   <si>
     <t xml:space="preserve">  </t>
   </si>
+  <si>
+    <t>n=</t>
+  </si>
+  <si>
+    <t>∂E/∂W5 = (ao1-t1) * ao1*(1-ao1) * ah1</t>
+  </si>
+  <si>
+    <t>∂E/∂W6=(ao1-t1) * ao1*(1-ao1) * ah2</t>
+  </si>
+  <si>
+    <t>∂E/∂W7=(ao2-t2) * ao2*(1-ao2) * ah1</t>
+  </si>
+  <si>
+    <t>∂E/∂W8(ao2-t2) * ao2*(1-ao2) * ah2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">∂E/∂W1 = ((ao1-t1) * ao1 * (1-ao1)*w5*ah1*(1-ah1)*i1) + ((ao2-t2) * ao2 * (1-ao2)*w7*ah1*(1-ah1)*i1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">∂E/∂W2= ((ao1-t1) * ao1 * (1-ao1)*w5*ah1*(1-ah1)*i2) + ((ao2-t2) * ao2 * (1-ao2)*w7*ah1*(1-ah1)*i2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">∂E/∂W3= ((ao1-t1) * ao1 * (1-ao1)*w6*ah2*(1-ah2)*i1) + ((ao2-t2) * ao2 * (1-ao2)*w8*ah2*(1-ah2)*i1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">∂E/∂W4= ((ao1-t1) * ao1 * (1-ao1)*w6*ah2*(1-ah2)*i2) + ((ao2-t2) * ao2 * (1-ao2)*w8*ah2*(1-ah2)*i2) </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +206,12 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -3868,8 +3901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A677CD16-2D5C-4E7A-9BDE-9D5527AA442D}">
   <dimension ref="B3:AF100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="74" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3879,16 +3912,60 @@
     <col min="15" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="7:15" x14ac:dyDescent="0.3">
       <c r="L3" s="7"/>
     </row>
-    <row r="5" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="7:15" x14ac:dyDescent="0.3">
       <c r="N5" s="7"/>
       <c r="O5" s="2" t="s">
         <v>31</v>
       </c>
     </row>
+    <row r="16" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="G16" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="G17" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="G18" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="G19" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="E23" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="E24" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="E25" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="E26" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="30" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="J30" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="K30" s="2">
         <v>2</v>
       </c>
@@ -12277,6 +12354,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>